<commit_message>
fixes to ed parsers, #795
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg development.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Stock</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Destination</t>
+  </si>
+  <si>
+    <t>Crew</t>
   </si>
 </sst>
 </file>
@@ -398,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G3"/>
+  <dimension ref="A3:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -427,6 +430,9 @@
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix loading gif bugs
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg development.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
     <sheet name="Picking" sheetId="2" r:id="rId2"/>
-    <sheet name="HU Transfer" sheetId="3" r:id="rId3"/>
+    <sheet name="Shocking" sheetId="4" r:id="rId3"/>
+    <sheet name="HU Transfer" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>Stock</t>
   </si>
@@ -49,21 +50,12 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Pick Count</t>
-  </si>
-  <si>
-    <t>Pick Type</t>
-  </si>
-  <si>
     <t>Program</t>
   </si>
   <si>
     <t>Count</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Destination</t>
   </si>
   <si>
@@ -89,6 +81,18 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Tray</t>
+  </si>
+  <si>
+    <t>PICK TYPE</t>
+  </si>
+  <si>
+    <t>Match to choice in app</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
   </si>
 </sst>
 </file>
@@ -182,6 +186,8 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -191,9 +197,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,15 +480,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H3"/>
+  <dimension ref="A3:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -502,10 +515,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -516,18 +535,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H3"/>
+  <dimension ref="A2:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -547,13 +578,25 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -561,27 +604,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q3"/>
+  <dimension ref="A2:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:Q3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -601,42 +646,121 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add comments to Egg development parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-egg development.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-egg development.xlsx
@@ -26,8 +26,499 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mandatory, set equal to cross if needed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fecundity Photo Count, Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stoyel, Quentin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Match the column header to count code selected in app. Use as many columns as needed.  Value should be the counts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Match the column header to count code selected in app. Use as many columns as needed.  Value should be the counts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stoyel, Quentin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Match the column header to count code selected in app. Use as many columns as needed.  Value should be the counts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Match the column header to count code selected in app. Use as many columns as needed.  Value should be the counts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Mandatory set equal to cross if needed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. EQU, Bonell, Odell, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If filled, Trough col must be filled in as well</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Can be either a drawer (eg. 4.3) or a cup (eg. 4.3.1)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Set to Y if entire tray is moving and N/blank if only taking a selection of eggs from the tray. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Stock</t>
   </si>
@@ -87,9 +578,6 @@
   </si>
   <si>
     <t>PICK TYPE</t>
-  </si>
-  <si>
-    <t>Match to choice in app</t>
   </si>
   <si>
     <t>Weight (g)</t>
@@ -99,13 +587,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -188,6 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -195,9 +697,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -479,30 +978,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A3" sqref="A3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -530,15 +1028,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,20 +1051,14 @@
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="7"/>
-    </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -594,20 +1087,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,20 +1111,14 @@
     <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="7"/>
-    </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -662,20 +1147,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,21 +1178,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -731,7 +1214,7 @@
         <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
@@ -764,5 +1247,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>